<commit_message>
This IE feed works fine for 005 aggregation. Must check 049.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/EOL/EOL_RegionConcordance.xlsx
+++ b/ConcordanceLibrary/EOL/EOL_RegionConcordance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="145">
   <si>
     <t>Code</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Algeria</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Benin</t>
   </si>
   <si>
-    <t>Bermuda</t>
-  </si>
-  <si>
     <t>Bolivia</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>Ethiopia</t>
   </si>
   <si>
-    <t>Faeroe Islands</t>
-  </si>
-  <si>
     <t>Fiji</t>
   </si>
   <si>
@@ -366,9 +357,6 @@
     <t>Senegal</t>
   </si>
   <si>
-    <t>Kosovo</t>
-  </si>
-  <si>
     <t>Seychelles</t>
   </si>
   <si>
@@ -463,6 +451,9 @@
   </si>
   <si>
     <t>EOL</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -789,20 +780,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B246"/>
+  <dimension ref="A1:B222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -810,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -818,7 +812,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -826,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -834,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -842,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -850,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -858,7 +852,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -866,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -874,7 +868,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -882,7 +876,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -890,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -898,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -906,7 +900,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -914,7 +908,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -922,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -930,7 +924,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -938,7 +932,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -946,7 +940,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -954,7 +948,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -962,7 +956,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -970,7 +964,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -978,7 +972,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -986,7 +980,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -994,7 +988,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1002,7 +996,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1010,7 +1004,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1018,7 +1012,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1026,7 +1020,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1034,7 +1028,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1042,7 +1036,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1050,7 +1044,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1058,7 +1052,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1066,7 +1060,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1074,7 +1068,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1082,7 +1076,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1090,7 +1084,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1098,7 +1092,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1106,7 +1100,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1114,7 +1108,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1122,7 +1116,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1130,7 +1124,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1138,7 +1132,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1154,7 +1148,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1162,7 +1156,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1170,7 +1164,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1178,7 +1172,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1186,7 +1180,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1194,7 +1188,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1202,7 +1196,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1210,7 +1204,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1218,7 +1212,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1226,7 +1220,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1234,7 +1228,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1242,7 +1236,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1250,7 +1244,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1266,7 +1260,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1274,7 +1268,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1282,7 +1276,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1290,7 +1284,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1298,7 +1292,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1306,7 +1300,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -1314,7 +1308,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1322,7 +1316,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1330,7 +1324,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -1338,7 +1332,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1346,7 +1340,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -1354,7 +1348,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -1362,7 +1356,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1370,7 +1364,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -1378,7 +1372,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1386,7 +1380,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1394,7 +1388,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -1402,7 +1396,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1410,7 +1404,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -1418,7 +1412,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -1426,7 +1420,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -1442,7 +1436,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -1458,7 +1452,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -1466,7 +1460,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1474,7 +1468,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -1482,7 +1476,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -1490,7 +1484,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -1498,7 +1492,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -1506,7 +1500,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -1514,7 +1508,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -1522,7 +1516,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -1530,7 +1524,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -1538,7 +1532,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -1546,7 +1540,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -1554,7 +1548,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -1562,7 +1556,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -1570,7 +1564,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -1578,7 +1572,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -1586,7 +1580,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -1594,7 +1588,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -1602,7 +1596,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -1610,7 +1604,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -1618,7 +1612,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -1626,7 +1620,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -1634,7 +1628,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -1642,7 +1636,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -1650,7 +1644,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -1658,7 +1652,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -1666,7 +1660,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -1674,7 +1668,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -1682,7 +1676,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -1690,7 +1684,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -1698,7 +1692,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -1706,7 +1700,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -1714,7 +1708,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -1722,7 +1716,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -1730,7 +1724,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -1738,7 +1732,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>76</v>
+        <v>144</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -1746,7 +1740,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -1754,7 +1748,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -1762,7 +1756,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -1770,7 +1764,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -1778,7 +1772,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -1786,7 +1780,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -1794,7 +1788,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -1802,7 +1796,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -1810,7 +1804,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -1818,7 +1812,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
@@ -1826,7 +1820,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -1834,7 +1828,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -1842,7 +1836,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -1850,7 +1844,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -1858,7 +1852,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -1866,7 +1860,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -1874,7 +1868,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -1882,7 +1876,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -1890,7 +1884,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -1898,7 +1892,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -1906,7 +1900,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -1914,7 +1908,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -1922,7 +1916,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -1930,7 +1924,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -1938,7 +1932,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -1946,7 +1940,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -1954,7 +1948,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -1962,7 +1956,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -1970,7 +1964,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -1978,7 +1972,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -1986,7 +1980,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -1994,7 +1988,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -2002,7 +1996,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -2010,7 +2004,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -2018,7 +2012,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -2026,7 +2020,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -2034,7 +2028,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -2042,7 +2036,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -2050,7 +2044,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
@@ -2058,7 +2052,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -2066,7 +2060,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -2074,7 +2068,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -2082,7 +2076,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -2090,7 +2084,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -2098,7 +2092,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -2106,7 +2100,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -2114,7 +2108,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
@@ -2122,7 +2116,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -2130,7 +2124,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -2138,7 +2132,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -2146,7 +2140,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -2154,7 +2148,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
@@ -2162,7 +2156,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -2170,7 +2164,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -2178,7 +2172,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -2186,7 +2180,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -2194,7 +2188,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
@@ -2202,7 +2196,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -2210,7 +2204,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -2218,7 +2212,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -2226,7 +2220,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
@@ -2234,7 +2228,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -2242,7 +2236,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
@@ -2250,7 +2244,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -2258,7 +2252,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -2266,7 +2260,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -2274,7 +2268,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -2282,7 +2276,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -2290,7 +2284,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
@@ -2298,7 +2292,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -2306,7 +2300,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
@@ -2314,7 +2308,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
@@ -2322,7 +2316,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
@@ -2330,7 +2324,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
@@ -2338,7 +2332,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
@@ -2346,7 +2340,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -2354,7 +2348,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
@@ -2362,7 +2356,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
@@ -2370,7 +2364,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
@@ -2378,7 +2372,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
@@ -2386,7 +2380,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
@@ -2394,7 +2388,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -2402,7 +2396,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -2410,7 +2404,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
@@ -2418,7 +2412,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -2426,7 +2420,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
@@ -2434,7 +2428,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
@@ -2442,7 +2436,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
@@ -2450,7 +2444,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>4</v>
+        <v>135</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
@@ -2458,7 +2452,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
@@ -2466,7 +2460,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
@@ -2474,7 +2468,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
@@ -2482,7 +2476,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
@@ -2490,7 +2484,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
@@ -2498,7 +2492,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
@@ -2506,7 +2500,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
@@ -2514,7 +2508,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
@@ -2522,7 +2516,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
@@ -2530,7 +2524,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
@@ -2538,7 +2532,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
@@ -2546,7 +2540,7 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
@@ -2554,7 +2548,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
@@ -2562,7 +2556,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
@@ -2570,344 +2564,12 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A223">
-        <v>222</v>
-      </c>
-      <c r="B223" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A224">
-        <v>223</v>
-      </c>
-      <c r="B224" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A225">
-        <v>224</v>
-      </c>
-      <c r="B225" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A226">
-        <v>225</v>
-      </c>
-      <c r="B226" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A227">
-        <v>226</v>
-      </c>
-      <c r="B227" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A228">
-        <v>227</v>
-      </c>
-      <c r="B228" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A229">
-        <v>228</v>
-      </c>
-      <c r="B229" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A230">
-        <v>229</v>
-      </c>
-      <c r="B230" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A231">
-        <v>230</v>
-      </c>
-      <c r="B231" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A232">
-        <v>231</v>
-      </c>
-      <c r="B232" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A233">
-        <v>232</v>
-      </c>
-      <c r="B233" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A234">
-        <v>233</v>
-      </c>
-      <c r="B234" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A235">
-        <v>234</v>
-      </c>
-      <c r="B235" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A236">
-        <v>235</v>
-      </c>
-      <c r="B236" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A237">
-        <v>236</v>
-      </c>
-      <c r="B237" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A238">
-        <v>237</v>
-      </c>
-      <c r="B238" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239">
-        <v>238</v>
-      </c>
-      <c r="B239" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A240">
-        <v>239</v>
-      </c>
-      <c r="B240" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241">
-        <v>240</v>
-      </c>
-      <c r="B241" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A242">
-        <v>241</v>
-      </c>
-      <c r="B242" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243">
-        <v>242</v>
-      </c>
-      <c r="B243" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244">
-        <v>243</v>
-      </c>
-      <c r="B244" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245">
-        <v>244</v>
-      </c>
-      <c r="B245" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246">
-        <v>245</v>
-      </c>
-      <c r="B246" t="s">
-        <v>146</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B42">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B176">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B73">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B101">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B201">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B150">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B238">
     <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B211">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B212">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B191">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B215">
-    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2946,7 +2608,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B41 B43:B60 B177:B190 B63:B64 B74:B79 B81:B100 B102:B149 B202:B210 B151:B175 B239:B241 B213:B214 B192:B200 B66:B72 B216:B230 B232:B236 B243:B246">
+  <conditionalFormatting sqref="B239:B241 B223:B230 B232:B236 B243:B246">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>